<commit_message>
Add Check ons on expenses
</commit_message>
<xml_diff>
--- a/resources/template.xlsx
+++ b/resources/template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10107"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iestyngage/git/LabelTransaction/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iestyngage/git/LabelTransaction/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC8A3188-4F5E-E34C-BC1B-02C3639989D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C3A2CC-80CB-1D43-8CBC-9E549574B460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15560" xr2:uid="{CDBF9494-2178-B143-8977-F3547BA7C8A8}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>Expenses totals</t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t>Charity</t>
+  </si>
+  <si>
+    <t>Total of sums</t>
+  </si>
+  <si>
+    <t>Total values</t>
   </si>
 </sst>
 </file>
@@ -163,13 +169,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -484,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ECA96BA-F22C-C44F-BA74-BA6FC34C1910}">
-  <dimension ref="A1:O14"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection sqref="A1:B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -502,7 +507,7 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
+      <c r="B1" s="4"/>
       <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
@@ -513,19 +518,19 @@
         <v>2</v>
       </c>
       <c r="J1" s="3"/>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="M1" s="5"/>
-      <c r="N1" s="5"/>
-      <c r="O1" s="5"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -559,11 +564,12 @@
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>9</v>
+      <c r="A3">
+        <f>SUM(B5:B16)</f>
+        <v>0</v>
       </c>
       <c r="B3">
-        <f>SUMIF($G:$G,A3,$F:$F)</f>
+        <f>SUM(F3:F78)</f>
         <v>0</v>
       </c>
       <c r="I3" t="s">
@@ -575,115 +581,132 @@
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <f t="shared" ref="B4:B14" si="0">SUMIF($G:$G,A4,$F:$F)</f>
-        <v>0</v>
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
       </c>
       <c r="I4" t="s">
         <v>12</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J5" si="1">SUMIF($O:$O,I4,$N:$N)</f>
+        <f t="shared" ref="J4:J5" si="0">SUMIF($O:$O,I4,$N:$N)</f>
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="B5:B16" si="1">SUMIF($G:$G,A5,$F:$F)</f>
         <v>0</v>
       </c>
       <c r="I5" t="s">
         <v>14</v>
       </c>
       <c r="J5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B14">
-        <f t="shared" si="0"/>
+      <c r="B16">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add NA to template
</commit_message>
<xml_diff>
--- a/resources/template.xlsx
+++ b/resources/template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/iestyngage/git/LabelTransaction/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40C3A2CC-80CB-1D43-8CBC-9E549574B460}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86B13564-69EE-DE4B-A4DE-9DCB53D40EB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1180" yWindow="1500" windowWidth="27240" windowHeight="15560" xr2:uid="{CDBF9494-2178-B143-8977-F3547BA7C8A8}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>Expenses totals</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Total values</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -489,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ECA96BA-F22C-C44F-BA74-BA6FC34C1910}">
-  <dimension ref="A1:O16"/>
+  <dimension ref="A1:O17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B16"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -565,7 +568,7 @@
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
-        <f>SUM(B5:B16)</f>
+        <f>SUM(B5:B17)</f>
         <v>0</v>
       </c>
       <c r="B3">
@@ -591,7 +594,7 @@
         <v>12</v>
       </c>
       <c r="J4">
-        <f t="shared" ref="J4:J5" si="0">SUMIF($O:$O,I4,$N:$N)</f>
+        <f t="shared" ref="J4:J6" si="0">SUMIF($O:$O,I4,$N:$N)</f>
         <v>0</v>
       </c>
     </row>
@@ -600,7 +603,7 @@
         <v>9</v>
       </c>
       <c r="B5">
-        <f t="shared" ref="B5:B16" si="1">SUMIF($G:$G,A5,$F:$F)</f>
+        <f t="shared" ref="B5:B17" si="1">SUMIF($G:$G,A5,$F:$F)</f>
         <v>0</v>
       </c>
       <c r="I5" t="s">
@@ -619,6 +622,13 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="I6" t="s">
+        <v>26</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -706,6 +716,15 @@
         <v>23</v>
       </c>
       <c r="B16">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>

</xml_diff>